<commit_message>
Prepping for new tables
</commit_message>
<xml_diff>
--- a/Manuscript/Tables/SurfComplComp.xlsx
+++ b/Manuscript/Tables/SurfComplComp.xlsx
@@ -422,14 +422,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -453,7 +453,7 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>-5</v>
+        <v>-2.9</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
@@ -464,7 +464,7 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>4.9000000000000004</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C4" s="1">
         <f>0.000011/0.03</f>

</xml_diff>